<commit_message>
Update the work diray
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub_DATA\I_Shoes\Documentation\Journaux_de_travail\Romain Lenoir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub_DATA\I_Shoes_BDD\Documentation\Journaux_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FAE60B-7D99-4094-B4EA-D7483DE008CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6167A14E-9434-4A12-9C76-671E49DA4102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9075" yWindow="1905" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_de_travail" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -230,6 +230,12 @@
   <si>
     <t>Json data</t>
   </si>
+  <si>
+    <t>Mise à jour des pages de model</t>
+  </si>
+  <si>
+    <t>Change la méthodologie du site pour pouvoir inculquer l'appelation  des views dans le controllers</t>
+  </si>
 </sst>
 </file>
 
@@ -384,10 +390,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -736,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1502,7 @@
       <c r="G30" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1550,7 +1556,7 @@
       <c r="G32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="19" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1579,31 +1585,59 @@
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>45042</v>
+      </c>
+      <c r="B34" s="8">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="D34" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="13"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>45043</v>
+      </c>
+      <c r="B35" s="8">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.66736111111111107</v>
+      </c>
       <c r="D35" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="13"/>
+        <v>0.10347222222222219</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>

</xml_diff>